<commit_message>
Added examples for IF functions, AND, NOT
</commit_message>
<xml_diff>
--- a/testing_functions.xlsx
+++ b/testing_functions.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/excel_work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF10CCCD-76A9-C047-A7E1-2C51A63B07C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F89527C-6274-CA4C-BBA8-E04BA49B4BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0E1F609B-6B8B-6645-A592-C04F0F4286EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18400" windowHeight="16420" xr2:uid="{0E1F609B-6B8B-6645-A592-C04F0F4286EC}"/>
   </bookViews>
   <sheets>
     <sheet name="examples" sheetId="1" r:id="rId1"/>
-    <sheet name="array_challenges" sheetId="2" r:id="rId2"/>
+    <sheet name="transpose_testing" sheetId="2" r:id="rId2"/>
     <sheet name="thanks_rachelle" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -22,7 +22,7 @@
     <definedName name="date98">examples!$G$4</definedName>
     <definedName name="test">examples!$G$3</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
   <si>
     <t>11/02/1998</t>
   </si>
@@ -287,6 +287,27 @@
   </si>
   <si>
     <t>On 2nd sheet</t>
+  </si>
+  <si>
+    <t>Year Released</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>IFERROR</t>
+  </si>
+  <si>
+    <t>IFNA</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>NOT</t>
   </si>
 </sst>
 </file>
@@ -295,8 +316,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -537,7 +558,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -556,7 +577,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -576,10 +597,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -901,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5B230D-BC5E-1B4F-BD3B-912B3897C156}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,6 +938,7 @@
     <col min="6" max="6" width="23.1640625" customWidth="1"/>
     <col min="7" max="7" width="34.83203125" customWidth="1"/>
     <col min="8" max="8" width="29.1640625" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
@@ -939,7 +962,9 @@
       <c r="H2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="15"/>
+      <c r="I2" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -957,7 +982,9 @@
       <c r="H3" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3">
+        <v>1999</v>
+      </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -975,6 +1002,9 @@
       <c r="H4" t="s">
         <v>40</v>
       </c>
+      <c r="I4">
+        <v>1991</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -991,6 +1021,9 @@
       <c r="H5" t="s">
         <v>41</v>
       </c>
+      <c r="I5">
+        <v>1988</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -1006,6 +1039,9 @@
       <c r="H6" t="s">
         <v>42</v>
       </c>
+      <c r="I6">
+        <v>2012</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -1021,6 +1057,9 @@
       <c r="H7" t="s">
         <v>43</v>
       </c>
+      <c r="I7">
+        <v>2001</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -1036,6 +1075,9 @@
       <c r="H8" t="s">
         <v>44</v>
       </c>
+      <c r="I8">
+        <v>1993</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -1051,6 +1093,9 @@
       <c r="H9" t="s">
         <v>45</v>
       </c>
+      <c r="I9">
+        <v>1994</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -1060,8 +1105,14 @@
         <f>SEARCH("te?T",G3)</f>
         <v>11</v>
       </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
       <c r="H10" t="s">
         <v>46</v>
+      </c>
+      <c r="I10">
+        <v>2012</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="19" x14ac:dyDescent="0.25">
@@ -1072,6 +1123,10 @@
         <f>LEN(G3)</f>
         <v>31</v>
       </c>
+      <c r="G11" s="34" t="e">
+        <f>SUM(1,3,T)</f>
+        <v>#NAME?</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -1084,6 +1139,10 @@
       <c r="C12" t="s">
         <v>26</v>
       </c>
+      <c r="G12" t="e">
+        <f>VLOOKUP(I10,H2:I10,1)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -1134,7 +1193,7 @@
       </c>
       <c r="B17" s="8">
         <f ca="1">TODAY()</f>
-        <v>43746</v>
+        <v>43747</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.25">
@@ -1242,7 +1301,7 @@
       </c>
       <c r="B28" s="11">
         <f ca="1">NOW()</f>
-        <v>43746.665382291663</v>
+        <v>43747.411791087965</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="19" x14ac:dyDescent="0.25">
@@ -1323,14 +1382,72 @@
       <c r="A37" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="B37" t="str">
+        <f>VLOOKUP(G10,$H$2:$I$10,1,0)</f>
+        <v>School Daze</v>
+      </c>
     </row>
     <row r="38" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" t="b">
+        <f>IF(I3=1999, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" t="b">
+        <f>IFERROR(G11, TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="b">
+        <f>_xlfn.IFNA(G12, TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" t="b">
+        <f>IF(OR(H3="Deep Blue Sea", H8="Eve's Bayou"),TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" t="b">
+        <f>IF(AND(H3="Deep Blue Sea", H8="Eve's Bayou"),TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" t="str">
+        <f>IF(NOT(B42),"It's true!","It's false!")</f>
+        <v>It's true!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B38">
+      <c r="B44">
         <f ca="1">RAND()*(100-50)</f>
-        <v>21.155207474769107</v>
+        <v>24.615747442727105</v>
       </c>
     </row>
   </sheetData>
@@ -1343,7 +1460,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added math function examples
</commit_message>
<xml_diff>
--- a/testing_functions.xlsx
+++ b/testing_functions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/excel_work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F89527C-6274-CA4C-BBA8-E04BA49B4BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B206EF4-854A-6942-8AD7-2B28293D7A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18400" windowHeight="16420" xr2:uid="{0E1F609B-6B8B-6645-A592-C04F0F4286EC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0E1F609B-6B8B-6645-A592-C04F0F4286EC}"/>
   </bookViews>
   <sheets>
     <sheet name="examples" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
   <si>
     <t>11/02/1998</t>
   </si>
@@ -109,18 +109,6 @@
     <t>EOMONTH</t>
   </si>
   <si>
-    <t>9 months after F3</t>
-  </si>
-  <si>
-    <t>pulled out month value from F3</t>
-  </si>
-  <si>
-    <t>the amount of days between F3 and F4</t>
-  </si>
-  <si>
-    <t>made a date inputting values</t>
-  </si>
-  <si>
     <t>WEEKDAY</t>
   </si>
   <si>
@@ -130,9 +118,6 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>24 hour units, doesn't output 24 hour clock</t>
-  </si>
-  <si>
     <t>HOUR</t>
   </si>
   <si>
@@ -190,9 +175,6 @@
     <t>HYPERLINK</t>
   </si>
   <si>
-    <t>https://www.google.com/search?q=white+contacts&amp;oq=white+contacts&amp;aqs=chrome..69i57j0l4j69i60.1726j0j4&amp;sourceid=chrome&amp;ie=UTF-8</t>
-  </si>
-  <si>
     <t>MATCH</t>
   </si>
   <si>
@@ -308,6 +290,66 @@
   </si>
   <si>
     <t>NOT</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>SUMIF</t>
+  </si>
+  <si>
+    <t>SUMIFS</t>
+  </si>
+  <si>
+    <t>Made Up Genres</t>
+  </si>
+  <si>
+    <t>Drama</t>
+  </si>
+  <si>
+    <t>Drama/Western</t>
+  </si>
+  <si>
+    <t>Horror/Action</t>
+  </si>
+  <si>
+    <t>Drama/Romance</t>
+  </si>
+  <si>
+    <t>Dramedy</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Action/Comedy</t>
+  </si>
+  <si>
+    <t>SUMPRODUCT</t>
+  </si>
+  <si>
+    <t>ABS</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>TRUNC</t>
+  </si>
+  <si>
+    <t>COUNT</t>
+  </si>
+  <si>
+    <t>https://www.lynda.com</t>
   </si>
 </sst>
 </file>
@@ -319,7 +361,7 @@
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -385,6 +427,10 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -558,7 +604,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -568,9 +614,6 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -602,6 +645,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -923,25 +969,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5B230D-BC5E-1B4F-BD3B-912B3897C156}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.5" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
     <col min="6" max="6" width="23.1640625" customWidth="1"/>
     <col min="7" max="7" width="34.83203125" customWidth="1"/>
     <col min="8" max="8" width="29.1640625" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="21">
       <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
@@ -954,500 +1001,822 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="2" spans="1:10" s="11" customFormat="1" ht="21">
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="11" customFormat="1" ht="19">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="7" t="str">
+      <c r="B3" s="6" t="str">
         <f>LEFT(G3,9)</f>
         <v>this is a</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="6" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B3)</f>
+        <v>=LEFT(G3,9)</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I3">
         <v>1999</v>
       </c>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="J3" s="35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="19">
+      <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="str">
+      <c r="B4" s="6" t="str">
         <f>MID(G3, 10, 5)</f>
         <v xml:space="preserve"> test</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="6" t="str">
+        <f t="shared" ref="C4:C55" ca="1" si="0">_xlfn.FORMULATEXT(B4)</f>
+        <v>=MID(G3, 10, 5)</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I4">
         <v>1991</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="J4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="19">
+      <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="7" t="str">
+      <c r="B5" s="6" t="str">
         <f>RIGHT(G3,9)</f>
         <v xml:space="preserve">est test </v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=RIGHT(G3,9)</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I5">
         <v>1988</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="J5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="19">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="str">
         <f>UPPER(G3)</f>
         <v xml:space="preserve">THIS IS A TEST TESTY TEST TEST </v>
       </c>
-      <c r="G6" s="8">
+      <c r="C6" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=UPPER(G3)</v>
+      </c>
+      <c r="G6" s="7">
         <v>30000</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I6">
         <v>2012</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="J6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="19">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="str">
         <f>LOWER(B6)</f>
         <v xml:space="preserve">this is a test testy test test </v>
       </c>
-      <c r="G7" s="10">
+      <c r="C7" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=LOWER(B6)</v>
+      </c>
+      <c r="G7" s="9">
         <v>0.2714699074074074</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I7">
         <v>2001</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="J7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="19">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="str">
         <f>PROPER(G3)</f>
         <v xml:space="preserve">This Is A Test Testy Test Test </v>
       </c>
+      <c r="C8" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=PROPER(G3)</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I8">
         <v>1993</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="J8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="19">
+      <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B9">
         <f>FIND("test",G3)</f>
         <v>11</v>
       </c>
-      <c r="G9" t="s">
-        <v>50</v>
+      <c r="C9" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=FIND("test",G3)</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>103</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I9">
         <v>1994</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="J9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="19">
+      <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B10">
         <f>SEARCH("te?T",G3)</f>
         <v>11</v>
       </c>
+      <c r="C10" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SEARCH("te?T",G3)</v>
+      </c>
       <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" t="s">
         <v>41</v>
-      </c>
-      <c r="H10" t="s">
-        <v>46</v>
       </c>
       <c r="I10">
         <v>2012</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="J10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="19">
+      <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B11">
         <f>LEN(G3)</f>
         <v>31</v>
       </c>
-      <c r="G11" s="34" t="e">
+      <c r="C11" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=LEN(G3)</v>
+      </c>
+      <c r="G11" s="33" t="e">
         <f>SUM(1,3,T)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:10" ht="19">
+      <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <f>DATE(2019,12,31)</f>
         <v>43830</v>
       </c>
-      <c r="C12" t="s">
-        <v>26</v>
+      <c r="C12" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=DATE(2019,12,31)</v>
       </c>
       <c r="G12" t="e">
         <f>VLOOKUP(I10,H2:I10,1)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:10" ht="19">
+      <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B13">
         <f>DATEVALUE(G4)</f>
         <v>36101</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="C13" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=DATEVALUE(G4)</v>
+      </c>
+      <c r="G13">
+        <v>-27.81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="19">
+      <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <f>EDATE(G4,9)</f>
         <v>36374</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="C14" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=EDATE(G4,9)</v>
+      </c>
+      <c r="G14">
+        <v>27.81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="19">
+      <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="str">
         <f>DAY(G5)&amp;" is the day using F4, a text date"</f>
         <v>3 is the day using F4, a text date</v>
       </c>
-      <c r="C15" t="str">
-        <f>DAY(B13) &amp;" is the day using B8, a serial"</f>
-        <v>2 is the day using B8, a serial</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="C15" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=DAY(G5)&amp;" is the day using F4, a text date"</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="19">
+      <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B16">
         <f>_xlfn.DAYS(G5,G4)</f>
         <v>2132</v>
       </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="C16" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=DAYS(G5,G4)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="19">
+      <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <f ca="1">TODAY()</f>
         <v>43747</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="C17" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=TODAY()</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="19">
+      <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B18">
         <f>MONTH(G4)</f>
         <v>11</v>
       </c>
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="C18" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=MONTH(G4)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="19">
+      <c r="A19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <f>EOMONTH(G4,9)</f>
         <v>36403</v>
       </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="C19" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=EOMONTH(G4,9)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="19">
+      <c r="A20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B20">
         <f>YEAR(G6)</f>
         <v>1982</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>27</v>
+      <c r="C20" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=YEAR(G6)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="19">
+      <c r="A21" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B21">
         <f>WEEKDAY(B12)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>28</v>
+      <c r="C21" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=WEEKDAY(B12)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="19">
+      <c r="A22" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="B22">
         <f>WEEKNUM(G6)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="9">
+      <c r="C22" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=WEEKNUM(G6)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="19">
+      <c r="A23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="8">
         <f>TIME(13,40,55)</f>
         <v>0.57008101851851845</v>
       </c>
-      <c r="C23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>31</v>
+      <c r="C23" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=TIME(13,40,55)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="19">
+      <c r="A24" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B24">
         <f>HOUR(G7)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>32</v>
+      <c r="C24" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=HOUR(G7)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="19">
+      <c r="A25" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B25">
         <f>TIMEVALUE(G8)</f>
         <v>0.2714699074074074</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>34</v>
+      <c r="C25" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=TIMEVALUE(G8)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="19">
+      <c r="A26" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="B26">
         <f>MINUTE(G7)</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>35</v>
+      <c r="C26" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=MINUTE(G7)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="19">
+      <c r="A27" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B27">
         <f>SECOND(G7)</f>
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="11">
+      <c r="C27" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SECOND(G7)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="19">
+      <c r="A28" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="10">
         <f ca="1">NOW()</f>
-        <v>43747.411791087965</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>37</v>
+        <v>43747.43041724537</v>
+      </c>
+      <c r="C28" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=NOW()</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="19">
+      <c r="A29" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>47</v>
+        <v>75</v>
+      </c>
+      <c r="C29" s="6" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="19">
+      <c r="A30" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="B30">
         <f>COLUMN(date04)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>48</v>
+      <c r="C30" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=COLUMN(date04)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="19">
+      <c r="A31" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="B31">
         <f>COLUMNS(A1:G30)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="17" t="str">
-        <f>HYPERLINK("https://honeycolor.com/color-contact-lenses/zombie-white-screen-halloween-lens", "contacts")</f>
-        <v>contacts</v>
-      </c>
-      <c r="C32" s="17" t="str">
-        <f>HYPERLINK(G9,"google some contacts")</f>
-        <v>google some contacts</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>51</v>
+      <c r="C31" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=COLUMNS(A1:G30)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="19">
+      <c r="A32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="16" t="str">
+        <f>HYPERLINK(G9,"Online Courses")</f>
+        <v>Online Courses</v>
+      </c>
+      <c r="C32" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=HYPERLINK(G9,"Online Courses")</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="19">
+      <c r="A33" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B33">
         <f>MATCH(H3,H3:H10)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>52</v>
+      <c r="C33" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=MATCH(H3,H3:H10)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="19">
+      <c r="A34" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B34">
         <f>ROW(H10)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>53</v>
+      <c r="C34" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=ROW(H10)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="19">
+      <c r="A35" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B35">
         <f>ROWS(A1:C34)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>54</v>
+      <c r="C35" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=ROWS(A1:C34)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="19">
+      <c r="A36" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>55</v>
+        <v>76</v>
+      </c>
+      <c r="C36" s="6" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="19">
+      <c r="A37" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="B37" t="str">
         <f>VLOOKUP(G10,$H$2:$I$10,1,0)</f>
         <v>School Daze</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>84</v>
+      <c r="C37" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=VLOOKUP(G10,$H$2:$I$10,1,0)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="19">
+      <c r="A38" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="B38" t="b">
         <f>IF(I3=1999, TRUE, FALSE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>85</v>
+      <c r="C38" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=IF(I3=1999, TRUE, FALSE)</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="19">
+      <c r="A39" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="B39" t="b">
         <f>IFERROR(G11, TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>86</v>
+      <c r="C39" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=IFERROR(G11, TRUE)</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="19">
+      <c r="A40" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="B40" t="b">
         <f>_xlfn.IFNA(G12, TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>87</v>
+      <c r="C40" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=IFNA(G12, TRUE)</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="19">
+      <c r="A41" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="B41" t="b">
         <f>IF(OR(H3="Deep Blue Sea", H8="Eve's Bayou"),TRUE,FALSE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>88</v>
+      <c r="C41" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=IF(OR(H3="Deep Blue Sea", H8="Eve's Bayou"),TRUE,FALSE)</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="19">
+      <c r="A42" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="B42" t="b">
         <f>IF(AND(H3="Deep Blue Sea", H8="Eve's Bayou"),TRUE,FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>89</v>
+      <c r="C42" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=IF(AND(H3="Deep Blue Sea", H8="Eve's Bayou"),TRUE,FALSE)</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="19">
+      <c r="A43" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="B43" t="str">
         <f>IF(NOT(B42),"It's true!","It's false!")</f>
         <v>It's true!</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44">
+      <c r="C43" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=IF(NOT(B42),"It's true!","It's false!")</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="19">
+      <c r="A44" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C44" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=FALSE()</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="19">
+      <c r="A45" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C45" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=TRUE()</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="19">
+      <c r="A46" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46">
+        <f>SUM(I3:I10)</f>
+        <v>15990</v>
+      </c>
+      <c r="C46" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SUM(I3:I10)</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="19">
+      <c r="A47" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47">
+        <f>SUMIF(H3:H10,G10,I3:I10)</f>
+        <v>1988</v>
+      </c>
+      <c r="C47" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SUMIF(H3:H10,G10,I3:I10)</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="19">
+      <c r="A48" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48">
+        <f>SUMIFS(I3:I10, H3:H10, H4, J3:J10, J4)</f>
+        <v>1991</v>
+      </c>
+      <c r="C48" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SUMIFS(I3:I10, H3:H10, H4, J3:J10, J4)</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="19">
+      <c r="A49" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49">
+        <f>SUMPRODUCT(I3:I10)</f>
+        <v>15990</v>
+      </c>
+      <c r="C49" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SUMPRODUCT(I3:I10)</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="19">
+      <c r="A50" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50">
+        <f>ABS(G13)</f>
+        <v>27.81</v>
+      </c>
+      <c r="C50" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=ABS(G13)</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="19">
+      <c r="A51" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51">
+        <f>INT(G14)</f>
+        <v>27</v>
+      </c>
+      <c r="C51" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=INT(G14)</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="19">
+      <c r="A52" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52">
+        <f>MOD(G14,G15)</f>
+        <v>0.80999999999999872</v>
+      </c>
+      <c r="C52" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=MOD(G14,G15)</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="19">
+      <c r="A53" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53">
+        <f>TRUNC(G13,0)</f>
+        <v>-27</v>
+      </c>
+      <c r="C53" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=TRUNC(G13,0)</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="19">
+      <c r="A54" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54">
         <f ca="1">RAND()*(100-50)</f>
-        <v>24.615747442727105</v>
+        <v>24.319426050840043</v>
+      </c>
+      <c r="C54" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=RAND()*(100-50)</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="19">
+      <c r="A55" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55">
+        <f>COUNT(I2:I10)</f>
+        <v>8</v>
+      </c>
+      <c r="C55" s="6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=COUNT(I2:I10)</v>
       </c>
     </row>
   </sheetData>
@@ -1463,28 +1832,28 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="B1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1502,9 +1871,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>354</v>
@@ -1522,9 +1891,9 @@
         <v>98676</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>432</v>
@@ -1542,9 +1911,9 @@
         <v>2134</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>776</v>
@@ -1562,7 +1931,7 @@
         <v>98787</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="H9">
         <f t="array" ref="H9:M14">TRANSPOSE(A1:F5)</f>
         <v>0</v>
@@ -1583,7 +1952,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="H10" t="str">
         <v>header 1</v>
       </c>
@@ -1603,7 +1972,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>354</v>
       </c>
@@ -1626,7 +1995,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="H12" t="str">
         <v>header 3</v>
       </c>
@@ -1646,7 +2015,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="H13" t="str">
         <v>header 4</v>
       </c>
@@ -1666,7 +2035,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="H14" t="str">
         <v>header 5</v>
       </c>
@@ -1699,170 +2068,170 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="23"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
-      <c r="E3" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="26">
+    <row r="1" spans="1:10" ht="17" thickBot="1">
+      <c r="A1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="22"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="23"/>
+      <c r="E3" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="25">
         <v>1</v>
       </c>
-      <c r="J3" s="27"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
-      <c r="B4" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="29">
+      <c r="J3" s="26"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="23"/>
+      <c r="B4" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="28">
         <f>CHOOSE(VLOOKUP(B4,H3:I6,2,FALSE),SUM(F4:F11),AVERAGE(F4:F11),MAX(F4:F11),MIN(F4:F11))</f>
         <v>120</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="29">
+        <v>12</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="25">
+        <v>2</v>
+      </c>
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="23"/>
+      <c r="E5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="29">
+        <v>10</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="25">
+        <v>3</v>
+      </c>
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="23"/>
+      <c r="E6" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="29">
+        <v>15</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="25">
+        <v>4</v>
+      </c>
+      <c r="J6" s="26"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="23"/>
+      <c r="E7" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F7" s="29">
+        <v>18</v>
+      </c>
+      <c r="J7" s="26"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="23"/>
+      <c r="E8" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="29">
+        <v>17</v>
+      </c>
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="23"/>
+      <c r="E9" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="29">
+        <v>19</v>
+      </c>
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="23"/>
+      <c r="E10" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="29">
+        <v>17</v>
+      </c>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="23"/>
+      <c r="E11" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="29">
         <v>12</v>
       </c>
-      <c r="H4" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="26">
-        <v>2</v>
-      </c>
-      <c r="J4" s="27"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
-      <c r="E5" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="30">
-        <v>10</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" s="26">
-        <v>3</v>
-      </c>
-      <c r="J5" s="27"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
-      <c r="E6" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="30">
-        <v>15</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="I6" s="26">
-        <v>4</v>
-      </c>
-      <c r="J6" s="27"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
-      <c r="E7" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="30">
-        <v>18</v>
-      </c>
-      <c r="J7" s="27"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="E8" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="30">
-        <v>17</v>
-      </c>
-      <c r="J8" s="27"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="E9" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="30">
-        <v>19</v>
-      </c>
-      <c r="J9" s="27"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="E10" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="30">
-        <v>17</v>
-      </c>
-      <c r="J10" s="27"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="E11" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="30">
-        <v>12</v>
-      </c>
-      <c r="J11" s="27"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
-      <c r="J12" s="27"/>
-    </row>
-    <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="33"/>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="23"/>
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="1:10" ht="17" thickBot="1">
+      <c r="A13" s="30"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="32"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>